<commit_message>
fix: corrigir persistência no executável removendo --add-data
O problema era que o PyInstaller estava embutindo o banco dentro do exe,
causando dados novos não serem salvos entre execuções.

Mudança:
- Remover --add-data 'gestao_editais.db;.' de build.bat
- Colocar cópia do banco em dist/ para ser usado pelo exe
- Atualizar instruções de build

Agora o exe usa o banco_de_dados que está no mesmo diretório,
garantindo persistência total dos dados.
</commit_message>
<xml_diff>
--- a/teste/acompanhamento_2025-12.xlsx
+++ b/teste/acompanhamento_2025-12.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -601,7 +601,65 @@
       </c>
       <c r="N2" s="2" t="inlineStr">
         <is>
-          <t>2025-12-09 23:37:33</t>
+          <t>2025-12-09 09:46:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="20" customHeight="1">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>001_Recursos_proprios</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>000</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>0000000000000000</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>carlos</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr"/>
+      <c r="F3" s="2" t="inlineStr"/>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>mestrado</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>R$ 2.100.00</t>
+        </is>
+      </c>
+      <c r="I3" s="2" t="inlineStr">
+        <is>
+          <t>2025-04-05</t>
+        </is>
+      </c>
+      <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>2025-12</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="L3" s="2" t="inlineStr">
+        <is>
+          <t>444</t>
+        </is>
+      </c>
+      <c r="M3" s="2" t="n"/>
+      <c r="N3" s="2" t="inlineStr">
+        <is>
+          <t>2025-12-09 23:58:21</t>
         </is>
       </c>
     </row>

</xml_diff>